<commit_message>
more layout work done with added verison for seperate PCB box housing
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\PCB Box\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>A</t>
   </si>
@@ -92,22 +92,52 @@
     <t>I/O input</t>
   </si>
   <si>
-    <t>Connector 1</t>
-  </si>
-  <si>
-    <t>Connector 2</t>
-  </si>
-  <si>
-    <t>RS232 TX</t>
-  </si>
-  <si>
-    <t>RS232 RX</t>
-  </si>
-  <si>
-    <t>Can L</t>
-  </si>
-  <si>
-    <t>Can H</t>
+    <t>RPM GND</t>
+  </si>
+  <si>
+    <t>ISO. I/O</t>
+  </si>
+  <si>
+    <t>Isolated I/O</t>
+  </si>
+  <si>
+    <t>Connector 1 pinout</t>
+  </si>
+  <si>
+    <t>Connector 1 MCU pins</t>
+  </si>
+  <si>
+    <t>Connector 2 pinout</t>
+  </si>
+  <si>
+    <t>Connector 2 MCU pins</t>
+  </si>
+  <si>
+    <t>12V relay</t>
+  </si>
+  <si>
+    <t>GND relay</t>
+  </si>
+  <si>
+    <t>HB-INA</t>
+  </si>
+  <si>
+    <t>HB-EN1</t>
+  </si>
+  <si>
+    <t>HB-EN2</t>
+  </si>
+  <si>
+    <t>HB-INB</t>
+  </si>
+  <si>
+    <t>HB-PWM</t>
+  </si>
+  <si>
+    <t>HB-MD</t>
+  </si>
+  <si>
+    <t>GND HB</t>
   </si>
 </sst>
 </file>
@@ -162,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +241,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -247,21 +289,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -317,27 +344,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,303 +676,579 @@
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="O3" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="10"/>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="O9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="O11" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="O13" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="25"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="O3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="16"/>
-      <c r="O4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>2</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="O11" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>3</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>4</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="O13" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more work on layout
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>A</t>
   </si>
@@ -138,6 +138,72 @@
   </si>
   <si>
     <t>GND HB</t>
+  </si>
+  <si>
+    <t>3.3V travel</t>
+  </si>
+  <si>
+    <t>GND travel</t>
+  </si>
+  <si>
+    <t>Travel 1</t>
+  </si>
+  <si>
+    <t>Travel 2</t>
+  </si>
+  <si>
+    <t>Travel 3</t>
+  </si>
+  <si>
+    <t>Travel 4</t>
+  </si>
+  <si>
+    <t>DAC Vout</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>GND RS232</t>
+  </si>
+  <si>
+    <t>GND CAN</t>
+  </si>
+  <si>
+    <t>RS 232 TX</t>
+  </si>
+  <si>
+    <t>RS 232 RX</t>
+  </si>
+  <si>
+    <t>CAN Low</t>
+  </si>
+  <si>
+    <t>CAN High</t>
+  </si>
+  <si>
+    <t>RS 232</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>GND Chassy</t>
+  </si>
+  <si>
+    <t>ECU AUX 1</t>
+  </si>
+  <si>
+    <t>ECU AUX 2</t>
+  </si>
+  <si>
+    <t>Gsens</t>
+  </si>
+  <si>
+    <t>Yaw</t>
+  </si>
+  <si>
+    <t>BITE</t>
   </si>
 </sst>
 </file>
@@ -192,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +319,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -344,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -357,9 +441,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -372,6 +454,13 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,30 +743,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="13" width="11.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="4"/>
@@ -691,7 +769,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="22"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -731,7 +809,7 @@
       <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -739,23 +817,35 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="D3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>57</v>
+      </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="O3" s="16" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="O3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -763,21 +853,33 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="D4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="10"/>
       <c r="O4" s="3" t="s">
         <v>13</v>
@@ -787,46 +889,72 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="13"/>
+      <c r="D5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="12"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="D6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="K6" s="10"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="4"/>
@@ -840,7 +968,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="22"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -880,10 +1008,10 @@
       <c r="M9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="O9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="20" t="s">
+      <c r="Q9" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -901,8 +1029,8 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
       <c r="Q10" t="s">
         <v>24</v>
       </c>
@@ -921,10 +1049,13 @@
       <c r="I11" s="10"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="O11" s="18" t="s">
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="O11" s="16" t="s">
         <v>20</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -941,8 +1072,8 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -958,28 +1089,36 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="O13" s="19" t="s">
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="O13" s="17" t="s">
         <v>21</v>
       </c>
+      <c r="Q13" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O15" s="30" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="23"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1025,85 +1164,123 @@
         <v>1</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="G18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="15"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="10"/>
+      <c r="H19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>3</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="15"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="13"/>
+      <c r="H20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="K20" s="10"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="L20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>4</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="23"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1154,24 +1331,12 @@
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
@@ -1185,22 +1350,12 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1212,22 +1367,12 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -1239,16 +1384,12 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
further layout work done
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>A</t>
   </si>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>BITE</t>
+  </si>
+  <si>
+    <t>Ignition cut</t>
+  </si>
+  <si>
+    <t>Speed pot</t>
+  </si>
+  <si>
+    <t>BrakeP</t>
+  </si>
+  <si>
+    <t>BrakeP2</t>
+  </si>
+  <si>
+    <t>Vtemp</t>
+  </si>
+  <si>
+    <t>VTemp2</t>
+  </si>
+  <si>
+    <t>GearPosAn</t>
   </si>
 </sst>
 </file>
@@ -428,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -461,6 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,28 +845,36 @@
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
       <c r="O3" s="14" t="s">
         <v>12</v>
       </c>
@@ -859,28 +889,36 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="L4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="10"/>
       <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
@@ -895,28 +933,36 @@
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="H5" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -928,30 +974,32 @@
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="L6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
     </row>
     <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
@@ -1391,6 +1439,34 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
     </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E30" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
changed H-Bridge design for modular mount, more layout on TC
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>A</t>
   </si>
@@ -209,22 +209,25 @@
     <t>Ignition cut</t>
   </si>
   <si>
-    <t>Speed pot</t>
-  </si>
-  <si>
     <t>BrakeP</t>
   </si>
   <si>
     <t>BrakeP2</t>
   </si>
   <si>
-    <t>Vtemp</t>
-  </si>
-  <si>
     <t>VTemp2</t>
   </si>
   <si>
     <t>GearPosAn</t>
+  </si>
+  <si>
+    <t>VTemp</t>
+  </si>
+  <si>
+    <t>SpeedPos</t>
+  </si>
+  <si>
+    <t>Ign Cut</t>
   </si>
 </sst>
 </file>
@@ -766,7 +769,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,22 +858,22 @@
         <v>14</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>14</v>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
@@ -904,17 +907,17 @@
       <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>66</v>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>38</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>39</v>
@@ -948,17 +951,17 @@
       <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
+      <c r="I5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>38</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>39</v>
@@ -989,13 +992,17 @@
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="K6" s="14" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
more layout done to PCB
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\PCB Box\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\OneDrive\Dokumenter\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\PCB Box\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -98,9 +98,6 @@
     <t>ISO. I/O</t>
   </si>
   <si>
-    <t>Isolated I/O</t>
-  </si>
-  <si>
     <t>Connector 1 pinout</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>BITE</t>
   </si>
   <si>
-    <t>Ignition cut</t>
-  </si>
-  <si>
     <t>BrakeP</t>
   </si>
   <si>
@@ -228,12 +222,48 @@
   </si>
   <si>
     <t>Ign Cut</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>FuelTemp</t>
+  </si>
+  <si>
+    <t>Brake-pot</t>
+  </si>
+  <si>
+    <t>Gear Encode 1</t>
+  </si>
+  <si>
+    <t>Gear Encode 2</t>
+  </si>
+  <si>
+    <t>Clutch-pot</t>
+  </si>
+  <si>
+    <t>AUX 1</t>
+  </si>
+  <si>
+    <t>AUX 3</t>
+  </si>
+  <si>
+    <t>AUX 2</t>
+  </si>
+  <si>
+    <t>AUX 4</t>
+  </si>
+  <si>
+    <t>HB-CS</t>
+  </si>
+  <si>
+    <t>Oil Pressure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -465,11 +495,8 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -477,15 +504,62 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,6 +653,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -614,6 +705,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kontor">
@@ -766,22 +874,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="13" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="11.75" customWidth="1"/>
+    <col min="15" max="15" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>25</v>
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -794,9 +902,9 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="20"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -834,183 +942,177 @@
       <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="40"/>
+      <c r="G3" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="14" t="s">
+      <c r="J3" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="14" t="s">
+      <c r="D4" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="F5" s="40"/>
+      <c r="G5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="14" t="s">
+      <c r="H5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="G6" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
-        <v>26</v>
+    </row>
+    <row r="8" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1023,9 +1125,9 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="20"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1063,117 +1165,136 @@
       <c r="M9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="Q10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="39"/>
+      <c r="L10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="O11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="39"/>
+      <c r="G11" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="O13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q13" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O15" s="30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="23"/>
+      <c r="B13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="39"/>
+      <c r="O13" s="22"/>
+    </row>
+    <row r="16" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1218,30 +1339,40 @@
       <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>31</v>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>13</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1249,26 +1380,40 @@
       <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="6" t="s">
+      <c r="B19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="6"/>
       <c r="K19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1276,26 +1421,40 @@
       <c r="A20" s="2">
         <v>3</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>35</v>
+      <c r="B20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1303,39 +1462,59 @@
       <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="C21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="M21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="23"/>
+      <c r="A23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1386,12 +1565,12 @@
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
@@ -1405,12 +1584,12 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1422,12 +1601,12 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -1439,43 +1618,38 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E30" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E31" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>59</v>
+      <c r="B30" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting to finish the layout
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\OneDrive\Dokumenter\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\PCB Box\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\Version 2\PCB Box\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>A</t>
   </si>
@@ -92,9 +92,6 @@
     <t>I/O input</t>
   </si>
   <si>
-    <t>RPM GND</t>
-  </si>
-  <si>
     <t>ISO. I/O</t>
   </si>
   <si>
@@ -258,12 +255,84 @@
   </si>
   <si>
     <t>Oil Pressure</t>
+  </si>
+  <si>
+    <t>12V Mains</t>
+  </si>
+  <si>
+    <t>GND DAC</t>
+  </si>
+  <si>
+    <t>GND Gencode</t>
+  </si>
+  <si>
+    <t>3.3V Gencode</t>
+  </si>
+  <si>
+    <t>GND Aux 1</t>
+  </si>
+  <si>
+    <t>GND Aux 2</t>
+  </si>
+  <si>
+    <t>GND Aux 3</t>
+  </si>
+  <si>
+    <t>GND Aux 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3V BrakePot </t>
+  </si>
+  <si>
+    <t>3.3V ClutchPot</t>
+  </si>
+  <si>
+    <t>GND ClutchPot</t>
+  </si>
+  <si>
+    <t>GND BrakePot</t>
+  </si>
+  <si>
+    <t>GND FuelT</t>
+  </si>
+  <si>
+    <t>GND Gyro</t>
+  </si>
+  <si>
+    <t>12V Gyro</t>
+  </si>
+  <si>
+    <t>GND RPM</t>
+  </si>
+  <si>
+    <t>GND Vtemp</t>
+  </si>
+  <si>
+    <t>GND BrakeP2</t>
+  </si>
+  <si>
+    <t>GND Vtemp 2</t>
+  </si>
+  <si>
+    <t>GND BrakeP</t>
+  </si>
+  <si>
+    <t>3.3V GearPAn</t>
+  </si>
+  <si>
+    <t>GND GearPAn</t>
+  </si>
+  <si>
+    <t>3.3V SpeedP</t>
+  </si>
+  <si>
+    <t>GND SpeedP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,23 +722,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -705,23 +757,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kontor">
@@ -877,19 +912,19 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="13" width="11.75" customWidth="1"/>
-    <col min="15" max="15" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -954,35 +989,35 @@
         <v>18</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="D3" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>48</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>49</v>
       </c>
       <c r="F3" s="40"/>
       <c r="G3" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="I3" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="37" t="s">
-        <v>66</v>
-      </c>
       <c r="K3" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>37</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>12</v>
@@ -996,35 +1031,35 @@
         <v>15</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="40"/>
       <c r="G4" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="K4" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="31" t="s">
         <v>37</v>
-      </c>
-      <c r="L4" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>13</v>
@@ -1038,35 +1073,35 @@
         <v>16</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>45</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>46</v>
       </c>
       <c r="F5" s="40"/>
       <c r="G5" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>59</v>
-      </c>
       <c r="J5" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="31" t="s">
         <v>37</v>
-      </c>
-      <c r="L5" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1077,42 +1112,40 @@
         <v>17</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="D6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>14</v>
-      </c>
+      <c r="F6" s="39"/>
       <c r="G6" s="35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="K6" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="31" t="s">
         <v>37</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1175,25 +1208,25 @@
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>49</v>
       </c>
       <c r="F10" s="39"/>
       <c r="G10" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="39"/>
       <c r="L10" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="39"/>
     </row>
@@ -1206,21 +1239,21 @@
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
       <c r="L11" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M11" s="39"/>
     </row>
@@ -1236,18 +1269,18 @@
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
       <c r="G12" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="39"/>
       <c r="I12" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="39"/>
       <c r="L12" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" s="39"/>
     </row>
@@ -1260,28 +1293,28 @@
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>55</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
       <c r="L13" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M13" s="39"/>
       <c r="O13" s="22"/>
     </row>
     <row r="16" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -1340,40 +1373,38 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>13</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E18" s="40"/>
       <c r="F18" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1381,40 +1412,38 @@
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>14</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E19" s="39"/>
       <c r="F19" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="K19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1422,40 +1451,40 @@
         <v>3</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="L20" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M20" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1463,45 +1492,45 @@
         <v>4</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="K21" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -1636,16 +1665,16 @@
         <v>21</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creating images for Wiki dokumentation
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/Version 2/PCB Box/pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="148">
   <si>
     <t>A</t>
   </si>
@@ -62,15 +62,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>12V</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
     <t>RPM3</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>Travel 4</t>
   </si>
   <si>
-    <t>DAC Vout</t>
-  </si>
-  <si>
     <t>DAC</t>
   </si>
   <si>
@@ -167,12 +155,6 @@
     <t>RS 232 RX</t>
   </si>
   <si>
-    <t>CAN Low</t>
-  </si>
-  <si>
-    <t>CAN High</t>
-  </si>
-  <si>
     <t>RS 232</t>
   </si>
   <si>
@@ -342,6 +324,150 @@
   </si>
   <si>
     <t>GND Aux 7</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PE7</t>
+  </si>
+  <si>
+    <t>PE8</t>
+  </si>
+  <si>
+    <t>PE9</t>
+  </si>
+  <si>
+    <t>PE10</t>
+  </si>
+  <si>
+    <t>PE11</t>
+  </si>
+  <si>
+    <t>PE12</t>
+  </si>
+  <si>
+    <t>PE13</t>
+  </si>
+  <si>
+    <t>PE14</t>
+  </si>
+  <si>
+    <t>PE15</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>PD8</t>
+  </si>
+  <si>
+    <t>PD10</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
+    <t>PD14</t>
+  </si>
+  <si>
+    <t>PD13</t>
+  </si>
+  <si>
+    <t>PD11</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>PA9</t>
+  </si>
+  <si>
+    <t>PA8</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>PE6</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA2</t>
   </si>
 </sst>
 </file>
@@ -532,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -544,11 +670,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,9 +704,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -602,6 +723,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,22 +1049,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="M30" sqref="A1:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="13" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -944,9 +1087,13 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="11"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M1" s="4"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -981,186 +1128,198 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="25" t="s">
+      <c r="J4" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="25" t="s">
+      <c r="K4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M4" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="28" t="s">
+      <c r="B6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="M6" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N7" s="14"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1173,9 +1332,14 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M8" s="4"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1210,142 +1374,164 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="35" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N9" s="14"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="33"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="30"/>
+      <c r="L10" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="37"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="33"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="G11" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="M11" s="37"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="33"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" s="30"/>
+      <c r="L12" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="M12" s="37"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M13" s="33"/>
-      <c r="O13" s="16"/>
-    </row>
-    <row r="16" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="B13" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+    </row>
+    <row r="16" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1391,40 +1577,40 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>78</v>
-      </c>
       <c r="I18" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1432,37 +1618,37 @@
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>67</v>
+      <c r="G19" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1470,40 +1656,38 @@
         <v>3</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>84</v>
+        <v>49</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>41</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1511,58 +1695,58 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>77</v>
+        <v>94</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
+      <c r="A23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="13"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1608,30 +1792,30 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="31" t="s">
-        <v>75</v>
+        <v>112</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="28" t="s">
+        <v>115</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
+        <v>116</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+        <v>120</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
       <c r="L25" s="9" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -1641,31 +1825,31 @@
         <v>2</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="33"/>
+        <v>104</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="30"/>
       <c r="F26" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="31" t="s">
-        <v>67</v>
+        <v>117</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="28" t="s">
+        <v>113</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1673,86 +1857,84 @@
         <v>3</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="33"/>
+        <v>105</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="30"/>
       <c r="F27" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>41</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="6"/>
       <c r="J27" s="6" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>4</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="33"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="30"/>
       <c r="F28" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
+        <v>119</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="6" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
+        <v>124</v>
+      </c>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>49</v>
+      <c r="G30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>